<commit_message>
ooutput update 2025 august
</commit_message>
<xml_diff>
--- a/output/CodeSystem-MindfulnessSettingCS.xlsx
+++ b/output/CodeSystem-MindfulnessSettingCS.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/CodeSystem/mindfulness-setting</t>
+    <t>https://2rdoc.pt/fhir/CodeSystem/mindfulness-setting</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-24T12:30:11+00:00</t>
+    <t>2025-08-20T10:40:04+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Phase 3 Complete: ZERO errors and 67% warning reduction
Summary:
- Errors: 54 → 0 (-100%)
- Warnings: 365 → 120 (-67.1%)
- Info/Hints: 68 → 13 (-80.9%)

Phase 3.9-3.15: Error elimination
- Fixed element mismatches in Extensions
- Corrected cardinality constraints
- Resolved type mismatches

Phase 3.19-3.23: Warning reduction
- Created 6 new CodeSystems (MindfulnessTypesCS.fsh)
- Added caseSensitive to 13 CodeSystems for ShareableCodeSystem compliance
- Fixed SUSHI compilation errors
- Clean build with 0 broken links

Documentation: backups/Phase3_Complete_Results.md

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/CodeSystem-MindfulnessSettingCS.xlsx
+++ b/output/CodeSystem-MindfulnessSettingCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-02T11:12:29+01:00</t>
+    <t>2025-10-02T18:31:12+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>CodeSystem defining different settings where mindfulness practice can occur</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -456,72 +459,74 @@
       <c r="A17" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" t="s" s="2">
+        <v>28</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -539,75 +544,75 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2"/>
     </row>

</xml_diff>